<commit_message>
implemented the base functionality DC excel 2 DC json
</commit_message>
<xml_diff>
--- a/tests/test_datasets/invalid_dc_excel.xlsx
+++ b/tests/test_datasets/invalid_dc_excel.xlsx
@@ -70,7 +70,7 @@
     <t>nominal</t>
   </si>
   <si>
-    <t>{"AD","in"},{"MCI","MCI"},{"NL","NL"}</t>
+    <t>{"in","AD"},{"MCI","MCI"},{"NL","NL"}</t>
   </si>
   <si>
     <t>Variable_3</t>
@@ -79,7 +79,7 @@
     <t>variable_3</t>
   </si>
   <si>
-    <t>{"1","1.5T"},{"2","2,4"}</t>
+    <t>{"1,5","1.5T"},{"2","2,4"}</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
     <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="40.86214285714286" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>

</xml_diff>